<commit_message>
Some changes were left uncommited from sometime now, so decided to commit them
</commit_message>
<xml_diff>
--- a/Certificate Automation/certificate_data.xlsx
+++ b/Certificate Automation/certificate_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Aryan119\Codes\Python Coding\Young-Skilled-India\Certificate Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DE69F1-72FC-4ECF-BE52-0442C04E37D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F74B1B2-75CE-48B4-8572-24FD13408D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,25 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>S.No.</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>College</t>
-  </si>
-  <si>
-    <t>Duration</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,30 +33,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -77,34 +50,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -126,9 +77,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -166,9 +117,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,26 +152,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -253,26 +187,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -446,37 +363,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.5546875" defaultRowHeight="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>